<commit_message>
AAP-36 + AAP-34: Import and export
</commit_message>
<xml_diff>
--- a/html/modules/custom/iasc_service/bulk_template.xlsx
+++ b/html/modules/custom/iasc_service/bulk_template.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Services" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Services!$A$1:$M$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Services!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Updated</t>
   </si>
@@ -43,7 +43,10 @@
     <t xml:space="preserve">Service Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Service Coverage</t>
+    <t xml:space="preserve">Service Coverage Region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service Coverage Country</t>
   </si>
   <si>
     <t xml:space="preserve">Global Focal Point</t>
@@ -193,19 +196,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="4" style="0" width="21.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="4" style="0" width="21.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -242,13 +245,13 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
@@ -262,6 +265,9 @@
       </c>
       <c r="R1" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>